<commit_message>
* new proto file
</commit_message>
<xml_diff>
--- a/plan/excel/skill_技能表.xlsx
+++ b/plan/excel/skill_技能表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="SkillProto" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>作者</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -32,7 +32,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">：秒
+          <t xml:space="preserve">：毫秒
 </t>
         </r>
       </text>
@@ -133,7 +133,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -253,7 +253,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -402,7 +402,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -1074,7 +1074,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1090,7 +1090,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1380,20 +1380,20 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19:H29"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10:F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.875" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="10" width="23.75" customWidth="1"/>
-    <col min="11" max="11" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="23.36328125" customWidth="1"/>
+    <col min="10" max="10" width="23.7265625" customWidth="1"/>
+    <col min="11" max="11" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -1547,10 +1547,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1568,7 +1568,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1001</v>
       </c>
@@ -1582,10 +1582,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1603,7 +1603,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1001</v>
       </c>
@@ -1617,10 +1617,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1638,7 +1638,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1001</v>
       </c>
@@ -1652,10 +1652,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1673,7 +1673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1001</v>
       </c>
@@ -1687,10 +1687,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1708,7 +1708,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1002</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -1740,7 +1740,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1002</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -1772,7 +1772,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1002</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -1804,7 +1804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1002</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -1836,7 +1836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1002</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F14">
         <v>6</v>
@@ -1868,7 +1868,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1003</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -1900,7 +1900,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1003</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F16">
         <v>6</v>
@@ -1932,7 +1932,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1003</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -1964,7 +1964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1003</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -1996,7 +1996,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1003</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F19">
         <v>6</v>
@@ -2028,7 +2028,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1004</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -2060,7 +2060,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1004</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F21">
         <v>6</v>
@@ -2092,7 +2092,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1004</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F22">
         <v>6</v>
@@ -2124,7 +2124,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1004</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F23">
         <v>6</v>
@@ -2156,7 +2156,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1004</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -2188,7 +2188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1005</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F25">
         <v>6</v>
@@ -2220,7 +2220,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1005</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F26">
         <v>6</v>
@@ -2252,7 +2252,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1005</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F27">
         <v>6</v>
@@ -2282,7 +2282,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1005</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F28">
         <v>6</v>
@@ -2312,7 +2312,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1005</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>3000</v>
       </c>
       <c r="F29">
         <v>6</v>

</xml_diff>

<commit_message>
new battle: code voer
</commit_message>
<xml_diff>
--- a/plan/excel/skill_技能表.xlsx
+++ b/plan/excel/skill_技能表.xlsx
@@ -1933,10 +1933,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>jl</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>target_major</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2041,6 +2037,10 @@
   </si>
   <si>
     <t>80_2004_5</t>
+  </si>
+  <si>
+    <t>j</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2451,7 +2451,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2487,10 +2487,10 @@
         <v>53</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>18</v>
@@ -2499,7 +2499,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -2508,19 +2508,19 @@
         <v>63</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>13</v>
@@ -2558,10 +2558,10 @@
         <v>30</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>1</v>
@@ -2599,10 +2599,10 @@
         <v>55</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
@@ -2611,28 +2611,28 @@
         <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="M3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="O3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="Q3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>15</v>
@@ -2670,10 +2670,10 @@
         <v>31</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>12</v>
@@ -2971,10 +2971,10 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>43</v>
@@ -3023,10 +3023,10 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>44</v>
@@ -3075,10 +3075,10 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>45</v>
@@ -3127,10 +3127,10 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>46</v>
@@ -3179,10 +3179,10 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>47</v>
@@ -3231,10 +3231,10 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>40</v>
@@ -3274,10 +3274,10 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R17" s="3" t="s">
         <v>40</v>
@@ -3317,10 +3317,10 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>40</v>
@@ -3360,10 +3360,10 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>40</v>
@@ -3403,10 +3403,10 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
* exporter: empty field of array * find target
</commit_message>
<xml_diff>
--- a/plan/excel/skill_技能表.xlsx
+++ b/plan/excel/skill_技能表.xlsx
@@ -388,879 +388,39 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-我方：
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 0
- 1
- 2
- 3
- 4
- 5 // </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">以上为绝对位置
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 6 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">自己
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 7 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>自己所在排行</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>包括自己</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
- 8 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>自己所在列</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>包括自己</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
- 9 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>自己周围</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>包括自己</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
- 10 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>自己周围</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>不包括自己</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
- 11 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">已方第一排
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 12 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">乙方第二排行
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 13 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">乙方全体
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 14 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">已方第一列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 15 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">已方第二列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 16 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">已方第三列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 17 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>乙方</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>HP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">最少单位
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 18 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>乙方</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>HP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">百分比最少单位
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 101 // </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>定向寻找</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Id</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>，比如张飞、张苞</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>具体在另一张表中依次列表所有可能</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">敌方：
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 200 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>对面的第一个单位</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>简称目标</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
- 201 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对面的第二个单位
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 202 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对面的所有单位
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 203 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对方第一排
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 204 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对方第二排
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 205 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对方第一列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 206 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对方第二列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 207 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对方第三列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 208 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">对方全体
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 209 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">目标所在排
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 210 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">目标所在列
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 211 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">目标周边
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 212 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>敌方</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>HP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">最少
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 213 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>敌方</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>HP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">百分比最少
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 301 //</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>定向寻找</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Id</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>，（与</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>101</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>类似，寻找我的仇人，比如吕蒙喜欢找关羽杀）</t>
+已方：
+ 1 ~ 6 // 绝对位置
+ 7 自己所在排行(包括自己)
+ 8 自己所在列(包括自己)
+ 9 自己周围(包括自己)
+ 10 自己周围(不包括自己)
+ 11 已方第一排
+ 12 已方第二排行
+ 13 已方全体
+ 14 已方第一列
+ 15 已方第二列
+ 16 已方第三列
+ 17 乙方HP最少单位
+ 18 乙方HP百分比最少单位
+ 19  自己
+ 101 // 定向寻找Id，比如张飞、张苞(具体在另一张表中依次列表所有可能)
+敌方：
+ 201 ~ 106 // 绝对位置
+ 207 对面的第一个单位(简称目标)
+ 208 对面的第二个单位
+ 209 对面的所有单位
+ 210 对方第一排
+ 211 对方第二排
+ 212 对方第一列
+ 213 对方第二列
+ 214 对方第三列
+ 215 对方全体
+ 216 目标所在排
+ 217 目标所在列
+ 218 目标周边
+ 219 敌方HP最少
+ 220 敌方HP百分比最少
+  //定向寻找Id，（与101类似，寻找我的仇人，比如吕蒙喜欢找关羽杀）</t>
         </r>
       </text>
     </comment>
@@ -1662,7 +822,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="93">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2037,10 +1197,6 @@
   </si>
   <si>
     <t>80_2004_5</t>
-  </si>
-  <si>
-    <t>j</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2449,9 +1605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2558,10 +1714,10 @@
         <v>30</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
debug over for battle
</commit_message>
<xml_diff>
--- a/plan/excel/skill_技能表.xlsx
+++ b/plan/excel/skill_技能表.xlsx
@@ -523,7 +523,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="143">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -716,41 +716,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>2_100|4_10|5_20</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_110|4_15|5_25</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_120|4_20|5_30</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_130|4_25|5_35</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_140|4_30|5_40</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>1_10|2_20|3_30|4_4|5_5</t>
-  </si>
-  <si>
-    <t>1_20|2_22|3_40|4_6|5_10</t>
-  </si>
-  <si>
-    <t>1_30|2_24|3_50|4_8|5_15</t>
-  </si>
-  <si>
-    <t>1_40|2_25|3_60|4_10|5_20</t>
-  </si>
-  <si>
-    <t>1_50|2_26|3_70|4_12|5_25</t>
-  </si>
-  <si>
     <t>ICON</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -1101,10 +1066,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>追加当前本体（总攻击量）的百分比</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>追加当前基础（属性的base部份）的百分比</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -1118,6 +1079,80 @@
   </si>
   <si>
     <t>l</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_100|2_10</t>
+  </si>
+  <si>
+    <t>1_100|2_10</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_110|2_15</t>
+  </si>
+  <si>
+    <t>1_110|2_15</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_100|2_10</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_120|2_20</t>
+  </si>
+  <si>
+    <t>1_120|2_20</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_130|2_25</t>
+  </si>
+  <si>
+    <t>1_130|2_25</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_140|2_30</t>
+  </si>
+  <si>
+    <t>1_140|2_30</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加当前本体（总攻击量）的百分比  这里填写整数，30代表30%</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(未实现</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>(未实现)4</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1527,9 +1562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R14" sqref="R14"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1568,13 +1603,13 @@
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>17</v>
@@ -1583,40 +1618,40 @@
         <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>13</v>
@@ -1636,7 +1671,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>1</v>
@@ -1681,13 +1716,13 @@
         <v>10</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.15">
@@ -1704,13 +1739,13 @@
         <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>19</v>
@@ -1719,40 +1754,40 @@
         <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>14</v>
@@ -1772,7 +1807,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>6</v>
@@ -1793,7 +1828,7 @@
         <v>12</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>11</v>
@@ -1805,7 +1840,7 @@
         <v>12</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>11</v>
@@ -1817,7 +1852,7 @@
         <v>12</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>12</v>
@@ -1840,7 +1875,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1863,13 +1898,13 @@
         <v>0.5</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -1892,7 +1927,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1938,7 +1973,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1984,7 +2019,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -2030,7 +2065,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -2076,7 +2111,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -2122,7 +2157,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -2140,27 +2175,27 @@
         <v>1</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="3">
         <v>0.85</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="3">
         <v>0.55000000000000004</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -2182,7 +2217,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2200,27 +2235,27 @@
         <v>1</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="3">
         <v>1</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="3">
         <v>0.6</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -2242,7 +2277,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2260,27 +2295,27 @@
         <v>1</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="3">
         <v>1.1499999999999999</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="3">
         <v>0.65</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>44</v>
+        <v>135</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -2302,7 +2337,7 @@
         <v>26</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -2320,27 +2355,27 @@
         <v>1</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="3">
         <v>1.3</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="3">
         <v>0.7</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -2362,7 +2397,7 @@
         <v>26</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2380,27 +2415,27 @@
         <v>1</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="3">
         <v>1.45</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>46</v>
+        <v>138</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="3">
         <v>0.75</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
@@ -2422,7 +2457,7 @@
         <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -2440,15 +2475,15 @@
         <v>2</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="L16" s="2"/>
       <c r="O16" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="P16" s="2"/>
       <c r="S16" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -2470,7 +2505,7 @@
         <v>26</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -2488,15 +2523,15 @@
         <v>2</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="L17" s="2"/>
       <c r="O17" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="P17" s="2"/>
       <c r="S17" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
@@ -2518,7 +2553,7 @@
         <v>26</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2536,15 +2571,15 @@
         <v>2</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="L18" s="2"/>
       <c r="O18" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="P18" s="2"/>
       <c r="S18" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
@@ -2566,7 +2601,7 @@
         <v>26</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2584,15 +2619,15 @@
         <v>2</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L19" s="2"/>
       <c r="O19" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="P19" s="2"/>
       <c r="S19" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
@@ -2614,7 +2649,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2632,15 +2667,15 @@
         <v>2</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="L20" s="2"/>
       <c r="O20" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="P20" s="2"/>
       <c r="S20" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
@@ -2660,7 +2695,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2680,21 +2715,17 @@
       <c r="K21" s="3"/>
       <c r="L21" s="2"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="3"/>
-      <c r="R21" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="V21" s="3" t="s">
         <v>31</v>
@@ -2712,7 +2743,7 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2732,21 +2763,17 @@
       <c r="K22" s="3"/>
       <c r="L22" s="2"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="V22" s="3" t="s">
         <v>31</v>
@@ -2764,7 +2791,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2784,21 +2811,17 @@
       <c r="K23" s="3"/>
       <c r="L23" s="2"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="3"/>
-      <c r="R23" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="U23" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="V23" s="3" t="s">
         <v>31</v>
@@ -2816,7 +2839,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2836,21 +2859,17 @@
       <c r="K24" s="3"/>
       <c r="L24" s="2"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="3"/>
-      <c r="R24" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="V24" s="3" t="s">
         <v>31</v>
@@ -2868,7 +2887,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2888,21 +2907,17 @@
       <c r="K25" s="3"/>
       <c r="L25" s="2"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="3"/>
-      <c r="R25" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="V25" s="3" t="s">
         <v>31</v>
@@ -2921,7 +2936,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2933,68 +2948,68 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B2" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C5" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
@@ -3002,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -3010,31 +3025,31 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B22">
-        <v>3</v>
+      <c r="B22" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B23" s="3">
-        <v>4</v>
+      <c r="B23" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>